<commit_message>
Created nested loops to run all model variations
Currently this code is in the "Creating factor analysis loop" script. Will integrate into the factor analysis script next
</commit_message>
<xml_diff>
--- a/R/LCAS conditional probabilities - all CAMs.xlsx
+++ b/R/LCAS conditional probabilities - all CAMs.xlsx
@@ -8,26 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED74ABD2-B8DE-45C4-AFED-720DE2EF6CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFC296C-FED2-41A8-B9F7-E962E2D8FC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{14232693-5FA9-4C18-9324-76C2FB7FD146}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="4" xr2:uid="{14232693-5FA9-4C18-9324-76C2FB7FD146}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Two Classes" sheetId="1" r:id="rId1"/>
+    <sheet name="Three Classes" sheetId="2" r:id="rId2"/>
+    <sheet name="Four Classes" sheetId="3" r:id="rId3"/>
+    <sheet name="Five Classes" sheetId="4" r:id="rId4"/>
+    <sheet name="Six Classes" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$F$1</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$A$2:$A$16</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$B$2:$B$16</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet2!$C$2:$C$16</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet2!$D$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet2!$D$2:$D$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Five Classes'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -432,7 +425,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'Two Classes'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -467,7 +460,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$16</c:f>
+              <c:f>'Two Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -520,7 +513,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$16</c:f>
+              <c:f>'Two Classes'!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -584,7 +577,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'Two Classes'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -619,7 +612,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$16</c:f>
+              <c:f>'Two Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -672,7 +665,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$16</c:f>
+              <c:f>'Two Classes'!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -989,7 +982,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$1</c:f>
+              <c:f>'Three Classes'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1024,7 +1017,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$2:$A$16</c:f>
+              <c:f>'Three Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -1077,7 +1070,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$16</c:f>
+              <c:f>'Three Classes'!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1141,7 +1134,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$1</c:f>
+              <c:f>'Three Classes'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1176,7 +1169,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$2:$A$16</c:f>
+              <c:f>'Three Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -1229,7 +1222,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$2:$C$16</c:f>
+              <c:f>'Three Classes'!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1293,7 +1286,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$1</c:f>
+              <c:f>'Three Classes'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1328,7 +1321,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$2:$A$16</c:f>
+              <c:f>'Three Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -1381,7 +1374,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$16</c:f>
+              <c:f>'Three Classes'!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1698,7 +1691,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$B$1</c:f>
+              <c:f>'Four Classes'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1733,7 +1726,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$A$2:$A$16</c:f>
+              <c:f>'Four Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -1786,7 +1779,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$2:$B$16</c:f>
+              <c:f>'Four Classes'!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1850,7 +1843,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$C$1</c:f>
+              <c:f>'Four Classes'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1885,7 +1878,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$A$2:$A$16</c:f>
+              <c:f>'Four Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -1938,7 +1931,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$C$2:$C$16</c:f>
+              <c:f>'Four Classes'!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2002,7 +1995,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$D$1</c:f>
+              <c:f>'Four Classes'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2037,7 +2030,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$A$2:$A$16</c:f>
+              <c:f>'Four Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -2090,7 +2083,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$D$2:$D$16</c:f>
+              <c:f>'Four Classes'!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2154,7 +2147,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$E$1</c:f>
+              <c:f>'Four Classes'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2189,7 +2182,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$A$2:$A$16</c:f>
+              <c:f>'Four Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -2242,7 +2235,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$E$2:$E$16</c:f>
+              <c:f>'Four Classes'!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2559,7 +2552,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$B$1</c:f>
+              <c:f>'Five Classes'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2594,7 +2587,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$A$2:$A$16</c:f>
+              <c:f>'Five Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -2647,7 +2640,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$2:$B$16</c:f>
+              <c:f>'Five Classes'!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2711,7 +2704,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$C$1</c:f>
+              <c:f>'Five Classes'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2746,7 +2739,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$A$2:$A$16</c:f>
+              <c:f>'Five Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -2799,7 +2792,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$C$2:$C$16</c:f>
+              <c:f>'Five Classes'!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2863,7 +2856,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$D$1</c:f>
+              <c:f>'Five Classes'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2898,7 +2891,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$A$2:$A$16</c:f>
+              <c:f>'Five Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -2951,7 +2944,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$D$2:$D$16</c:f>
+              <c:f>'Five Classes'!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3015,7 +3008,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$E$1</c:f>
+              <c:f>'Five Classes'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3050,7 +3043,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$A$2:$A$16</c:f>
+              <c:f>'Five Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -3103,7 +3096,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$E$2:$E$16</c:f>
+              <c:f>'Five Classes'!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3167,7 +3160,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$F$1</c:f>
+              <c:f>'Five Classes'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3202,7 +3195,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet4!$A$2:$A$16</c:f>
+              <c:f>'Five Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -3255,7 +3248,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$F$2:$F$16</c:f>
+              <c:f>'Five Classes'!$F$2:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3572,7 +3565,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$B$1</c:f>
+              <c:f>'Six Classes'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3607,7 +3600,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$2:$A$16</c:f>
+              <c:f>'Six Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -3660,7 +3653,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$B$2:$B$16</c:f>
+              <c:f>'Six Classes'!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3724,7 +3717,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$C$1</c:f>
+              <c:f>'Six Classes'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3759,7 +3752,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$2:$A$16</c:f>
+              <c:f>'Six Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -3812,7 +3805,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$C$2:$C$16</c:f>
+              <c:f>'Six Classes'!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3876,7 +3869,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$D$1</c:f>
+              <c:f>'Six Classes'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3911,7 +3904,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$2:$A$16</c:f>
+              <c:f>'Six Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -3964,7 +3957,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$D$2:$D$16</c:f>
+              <c:f>'Six Classes'!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -4028,7 +4021,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$E$1</c:f>
+              <c:f>'Six Classes'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4063,7 +4056,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$2:$A$16</c:f>
+              <c:f>'Six Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -4116,7 +4109,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$E$2:$E$16</c:f>
+              <c:f>'Six Classes'!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -4180,7 +4173,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$F$1</c:f>
+              <c:f>'Six Classes'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4215,7 +4208,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$2:$A$16</c:f>
+              <c:f>'Six Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -4268,7 +4261,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$F$2:$F$16</c:f>
+              <c:f>'Six Classes'!$F$2:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -4332,7 +4325,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$G$1</c:f>
+              <c:f>'Six Classes'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4367,7 +4360,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$2:$A$16</c:f>
+              <c:f>'Six Classes'!$A$2:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -4420,7 +4413,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$G$2:$G$16</c:f>
+              <c:f>'Six Classes'!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -7904,7 +7897,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A16"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8108,7 +8101,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0">
-      <selection sqref="A1:A16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8669,7 +8662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6593A61B-F7D7-4C70-B9B8-D71ED366397D}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+    <sheetView zoomScale="143" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -9031,7 +9024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C0EDBF-2099-43D8-B04E-72126FE2586B}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>